<commit_message>
GITBOOK-241: change request with no subject merged in GitBook
</commit_message>
<xml_diff>
--- a/.gitbook/assets/Buggy Component List (1) (1) (1).xlsx
+++ b/.gitbook/assets/Buggy Component List (1) (1) (1).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{025981CA-3542-462C-909D-863FEAE27501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D226A48A-BA41-42B9-A734-0328BCC1CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>Buggy components list</t>
   </si>
@@ -220,12 +220,6 @@
   </si>
   <si>
     <t>M5 nut</t>
-  </si>
-  <si>
-    <t>M3-10mm nylon Screw</t>
-  </si>
-  <si>
-    <t>M3 nylon nut</t>
   </si>
   <si>
     <t>Prints</t>
@@ -780,8 +774,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CustomerList" displayName="CustomerList" ref="B4:F60" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="B4:F60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CustomerList" displayName="CustomerList" ref="B4:F59" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="B4:F59" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Components" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Units ()" dataDxfId="3"/>
@@ -1029,10 +1023,10 @@
     <tabColor theme="6" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="30" customHeight="1"/>
@@ -1499,7 +1493,7 @@
         <v>51</v>
       </c>
       <c r="C32" s="17">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
@@ -1625,12 +1619,8 @@
       <c r="F41" s="17"/>
     </row>
     <row r="42" spans="2:6" ht="30" customHeight="1">
-      <c r="B42" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="17">
-        <v>4</v>
-      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
         <v>52</v>
@@ -1638,30 +1628,28 @@
       <c r="F42" s="17"/>
     </row>
     <row r="43" spans="2:6" ht="30" customHeight="1">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+    </row>
+    <row r="44" spans="2:6" ht="30" customHeight="1">
+      <c r="B44" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="17">
-        <v>4</v>
-      </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="17"/>
-    </row>
-    <row r="44" spans="2:6" ht="30" customHeight="1">
-      <c r="B44" s="22" t="s">
+      <c r="C44" s="17">
+        <v>1</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="2:6" ht="30" customHeight="1">
+      <c r="B45" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="2:6" ht="30" customHeight="1">
-      <c r="B45" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="C45" s="17">
         <v>1</v>
@@ -1672,7 +1660,7 @@
     </row>
     <row r="46" spans="2:6" ht="30" customHeight="1">
       <c r="B46" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="17">
         <v>1</v>
@@ -1683,10 +1671,10 @@
     </row>
     <row r="47" spans="2:6" ht="30" customHeight="1">
       <c r="B47" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -1694,7 +1682,7 @@
     </row>
     <row r="48" spans="2:6" ht="30" customHeight="1">
       <c r="B48" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" s="17">
         <v>2</v>
@@ -1705,7 +1693,7 @@
     </row>
     <row r="49" spans="2:6" ht="30" customHeight="1">
       <c r="B49" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" s="17">
         <v>2</v>
@@ -1716,7 +1704,7 @@
     </row>
     <row r="50" spans="2:6" ht="30" customHeight="1">
       <c r="B50" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="17">
         <v>2</v>
@@ -1727,10 +1715,10 @@
     </row>
     <row r="51" spans="2:6" ht="30" customHeight="1">
       <c r="B51" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
@@ -1738,7 +1726,7 @@
     </row>
     <row r="52" spans="2:6" ht="30" customHeight="1">
       <c r="B52" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" s="17">
         <v>4</v>
@@ -1749,10 +1737,10 @@
     </row>
     <row r="53" spans="2:6" ht="30" customHeight="1">
       <c r="B53" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
@@ -1760,7 +1748,7 @@
     </row>
     <row r="54" spans="2:6" ht="30" customHeight="1">
       <c r="B54" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" s="17">
         <v>1</v>
@@ -1771,7 +1759,7 @@
     </row>
     <row r="55" spans="2:6" ht="30" customHeight="1">
       <c r="B55" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C55" s="17">
         <v>1</v>
@@ -1782,7 +1770,7 @@
     </row>
     <row r="56" spans="2:6" ht="30" customHeight="1">
       <c r="B56" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
@@ -1793,7 +1781,7 @@
     </row>
     <row r="57" spans="2:6" ht="30" customHeight="1">
       <c r="B57" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="17">
         <v>1</v>
@@ -1804,7 +1792,7 @@
     </row>
     <row r="58" spans="2:6" ht="30" customHeight="1">
       <c r="B58" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="17">
         <v>1</v>
@@ -1815,7 +1803,7 @@
     </row>
     <row r="59" spans="2:6" ht="30" customHeight="1">
       <c r="B59" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" s="17">
         <v>1</v>
@@ -1825,71 +1813,60 @@
       <c r="F59" s="17"/>
     </row>
     <row r="60" spans="2:6" ht="30" customHeight="1">
-      <c r="B60" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" s="17">
-        <v>1</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
     </row>
     <row r="61" spans="2:6" ht="30" customHeight="1">
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
     </row>
     <row r="62" spans="2:6" ht="30" customHeight="1">
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
     </row>
     <row r="63" spans="2:6" ht="30" customHeight="1">
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" spans="2:6" ht="30" customHeight="1">
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
     </row>
     <row r="65" spans="2:6" ht="30" customHeight="1">
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
     </row>
     <row r="66" spans="2:6" ht="30" customHeight="1">
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
     </row>
     <row r="67" spans="2:6" ht="30" customHeight="1">
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-    </row>
-    <row r="68" spans="2:6" ht="30" customHeight="1">
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1937,15 +1914,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2257,6 +2225,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2278,11 +2255,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F9FC5B-1419-41E5-B909-94EB8B44A792}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11600A7-1852-41A2-85E0-7A283C2047C4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11600A7-1852-41A2-85E0-7A283C2047C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F9FC5B-1419-41E5-B909-94EB8B44A792}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>